<commit_message>
Create  folders for each teammember in milestone3
</commit_message>
<xml_diff>
--- a/planning/Group Project Timeline PG Group 6.xlsx
+++ b/planning/Group Project Timeline PG Group 6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhubowen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10917\Desktop\web_practice\25S1_WDC_PG_Groups_6\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852E0640-EEBC-8A4A-A618-4950426A6747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8AA1AA-D8DD-4189-A189-DE9FAA129E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="820" windowWidth="27780" windowHeight="17180" xr2:uid="{2F1AC7ED-6F65-BC40-8BC4-53273E012C28}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{2F1AC7ED-6F65-BC40-8BC4-53273E012C28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Group Project Milestone</t>
   </si>
@@ -50,114 +39,145 @@
     <t>All</t>
   </si>
   <si>
-    <t>API integration test, database schema</t>
-  </si>
-  <si>
     <t>Jie Li</t>
   </si>
   <si>
-    <t>UI mockups, search &amp; detail page</t>
-  </si>
-  <si>
     <t>Xinchen Luo</t>
   </si>
   <si>
-    <t>Game save functionality, custom fields</t>
-  </si>
-  <si>
-    <t>User dashboard, data visualization</t>
+    <t>Final report and demo submission</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Project Title</t>
+  </si>
+  <si>
+    <t>GameScape: Personalized Video Game Discovery and Journal</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Until 13/6/2025(week13)</t>
+  </si>
+  <si>
+    <t>Decide on project direction and concept (research APIs)</t>
+  </si>
+  <si>
+    <t>Create project proposal (title, description, API plan, database plan, user services</t>
+  </si>
+  <si>
+    <t>Discuss and refine proposal content</t>
+  </si>
+  <si>
+    <t>Develop collaboration plan (task division, communication methods, communication tools)</t>
+  </si>
+  <si>
+    <t>Create project development timeline</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Form project group and assign roles</t>
+  </si>
+  <si>
+    <t>Milestone 1：Project Planning</t>
+  </si>
+  <si>
+    <t>Milestone 2：Backend Setup, Frontend Design, Core Features</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Xinchen Luo, Jie Li, Xiyuan Zhang, Bowen Zhu</t>
+  </si>
+  <si>
+    <t>Completed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Xiyuan Zhang</t>
-  </si>
-  <si>
-    <t>QA, bug fixes, UI enhancements</t>
-  </si>
-  <si>
-    <t>Final report and demo submission</t>
-  </si>
-  <si>
-    <t>Due Date</t>
-  </si>
-  <si>
-    <t>Project Title</t>
-  </si>
-  <si>
-    <t>GameScape: Personalized Video Game Discovery and Journal</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Responsible</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Until 13/6/2025(week13)</t>
-  </si>
-  <si>
-    <t>Decide on project direction and concept (research APIs)</t>
-  </si>
-  <si>
-    <t>Create project proposal (title, description, API plan, database plan, user services</t>
-  </si>
-  <si>
-    <t>Discuss and refine proposal content</t>
-  </si>
-  <si>
-    <t>Develop collaboration plan (task division, communication methods, communication tools)</t>
-  </si>
-  <si>
-    <t>Create project development timeline</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Week</t>
-  </si>
-  <si>
-    <t>Deadline</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
-    <t>Form project group and assign roles</t>
-  </si>
-  <si>
-    <t>Milestone 1：Project Planning</t>
-  </si>
-  <si>
-    <t>Milestone 2：Backend Setup, Frontend Design, Core Features</t>
-  </si>
-  <si>
-    <t>Milestone 3：Profile &amp; Dashboard, Final Testing &amp; Polish, Submission</t>
-  </si>
-  <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>Xinchen Luo, Jie Li, Xiyuan Zhang, Bowen Zhu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xinchen Luo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>API integration test, backend server setting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Database schema, defined model relationships</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>implementing the user interface for game search, game detail display</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implement web core functionality(search, save games) overall project  debugging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Polish UI/UX for existing pages,build frontend for new features and enhance user feedback.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bowen Zhu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Develop backend APIs for advanced collection features (user notes, custom ratings, play status).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Jie Li </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extend database schema and Sequelize models for advanced collection details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project coordination, QA, and full-stack support, ensuring smooth integration of new features.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -171,7 +191,8 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -182,9 +203,15 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -231,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -368,11 +395,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -385,36 +423,74 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -422,50 +498,30 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -477,28 +533,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -830,30 +880,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05B9228-DB58-964E-B2E6-1877AE95D9A4}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="16" style="7" customWidth="1"/>
-    <col min="2" max="2" width="72.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="106.83203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="7" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="72.3046875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9.15234375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14.69140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="106.84375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="17.4609375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.84375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="20.4609375" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="10.84375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -861,12 +911,12 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
-        <v>14</v>
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="16" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
@@ -875,12 +925,12 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>34</v>
+    <row r="3" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -889,12 +939,12 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -903,7 +953,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -913,243 +963,295 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="B6" s="25"/>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="47">
+        <v>45768</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="33">
+        <v>4</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="35"/>
+      <c r="G9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="33">
+        <v>5</v>
+      </c>
+      <c r="D10" s="35"/>
+      <c r="E10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F10" s="35"/>
+      <c r="G10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="F11" s="35"/>
+      <c r="G11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="30"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="8">
+        <v>6</v>
+      </c>
+      <c r="D12" s="35"/>
+      <c r="E12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="11">
+        <v>7</v>
+      </c>
+      <c r="D13" s="48">
+        <v>45793</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="39"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="11">
+        <v>8</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="41"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="11">
+        <v>9</v>
+      </c>
+      <c r="D15" s="49"/>
+      <c r="E15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="11">
+        <v>10</v>
+      </c>
+      <c r="D16" s="50"/>
+      <c r="E16" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13">
+      <c r="G16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="13">
+        <v>11</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="43"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="13">
+        <v>11</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="43"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="13">
+        <v>11</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="E19" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="43"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="13">
+        <v>12</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="45"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="13">
+        <v>13</v>
+      </c>
+      <c r="D21" s="36"/>
+      <c r="E21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="46">
-        <v>45768</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19">
-        <v>4</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19">
-        <v>5</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="13">
-        <v>6</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25">
-        <v>7</v>
-      </c>
-      <c r="D13" s="45">
-        <v>45793</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="27"/>
-    </row>
-    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="25">
-        <v>8</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="27"/>
-    </row>
-    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="25">
-        <v>9</v>
-      </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="27"/>
-    </row>
-    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34">
-        <v>10</v>
-      </c>
-      <c r="D16" s="35">
-        <v>45821</v>
-      </c>
-      <c r="E16" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="34"/>
-      <c r="H16" s="36"/>
-    </row>
-    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="34">
-        <v>11</v>
-      </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="36"/>
-    </row>
-    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="34">
-        <v>12</v>
-      </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-    </row>
-    <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="41"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E22" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="F7:F12"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="D17:D21"/>
     <mergeCell ref="A13:B15"/>
-    <mergeCell ref="A16:B18"/>
+    <mergeCell ref="A17:B21"/>
     <mergeCell ref="D7:D12"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B12"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>